<commit_message>
Added second sheet for Create Standard parts from Excel
</commit_message>
<xml_diff>
--- a/Spreadsheet for Create Assembly From Excel & Create Standard Parts From Excel.xlsx
+++ b/Spreadsheet for Create Assembly From Excel & Create Standard Parts From Excel.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\iLogic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE0877E4-D7D3-4DD5-A2D3-BACC45806B0A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC1F53C-EF54-45BD-8250-F11D08E32335}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE0EA151-60DE-4798-A7EE-6788D2CE7F0D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{EE0EA151-60DE-4798-A7EE-6788D2CE7F0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -68,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>PDF name</t>
   </si>
@@ -177,13 +178,70 @@
   </si>
   <si>
     <t>Count of Occurrences (Assembly Only)</t>
+  </si>
+  <si>
+    <t>DRG NO.</t>
+  </si>
+  <si>
+    <t>Line1</t>
+  </si>
+  <si>
+    <t>Line2</t>
+  </si>
+  <si>
+    <t>Character Height</t>
+  </si>
+  <si>
+    <t>Dim A</t>
+  </si>
+  <si>
+    <t>Dim B</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>DT-123456-001</t>
+  </si>
+  <si>
+    <t>DT-123456-002</t>
+  </si>
+  <si>
+    <t>DT-123456-003</t>
+  </si>
+  <si>
+    <t>DT-123456-004</t>
+  </si>
+  <si>
+    <t>DT-123456-005</t>
+  </si>
+  <si>
+    <t>DT-123456-006</t>
+  </si>
+  <si>
+    <t>LOREM</t>
+  </si>
+  <si>
+    <t>IPSUM</t>
+  </si>
+  <si>
+    <t>DOLOR</t>
+  </si>
+  <si>
+    <t>SIT</t>
+  </si>
+  <si>
+    <t>AMET</t>
+  </si>
+  <si>
+    <t>CONSECTETUR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,6 +268,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -594,7 +658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{569F79E4-F061-4B08-827F-34BE4DD5DBE8}">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
@@ -735,4 +799,152 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{710B3DF5-992F-4C32-89E1-CAF50CAFA21D}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2">
+        <v>0.7</v>
+      </c>
+      <c r="E2">
+        <v>50</v>
+      </c>
+      <c r="F2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3">
+        <v>0.7</v>
+      </c>
+      <c r="E3">
+        <v>50</v>
+      </c>
+      <c r="F3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4">
+        <v>0.7</v>
+      </c>
+      <c r="E4">
+        <v>50</v>
+      </c>
+      <c r="F4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5">
+        <v>0.7</v>
+      </c>
+      <c r="E5">
+        <v>50</v>
+      </c>
+      <c r="F5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6">
+        <v>0.7</v>
+      </c>
+      <c r="E6">
+        <v>50</v>
+      </c>
+      <c r="F6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7">
+        <v>0.7</v>
+      </c>
+      <c r="E7">
+        <v>50</v>
+      </c>
+      <c r="F7">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>